<commit_message>
dinhtv7 fix phan quyen & ca thi
</commit_message>
<xml_diff>
--- a/public/assets/media/excel/Poetry-dowload-new.xlsx
+++ b/public/assets/media/excel/Poetry-dowload-new.xlsx
@@ -5,16 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mr.VanHau32\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Quang Vinh\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6792542B-F98F-4B30-B8B5-7529D162CADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEAD7E5C-182D-4753-9489-0C3B4E99275A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{1DBCA21E-12A4-472A-A2B4-C49F89FCDB90}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1DBCA21E-12A4-472A-A2B4-C49F89FCDB90}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Thông tin cơ sở" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
-  <si>
-    <t>#.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="23">
   <si>
     <t>Ngày thi</t>
   </si>
@@ -46,9 +42,6 @@
     <t>LỚP</t>
   </si>
   <si>
-    <t>Phát đề</t>
-  </si>
-  <si>
     <t>Toán</t>
   </si>
   <si>
@@ -58,52 +51,49 @@
     <t>VIE1026.05</t>
   </si>
   <si>
-    <t>Lý</t>
-  </si>
-  <si>
     <t>Hóa</t>
   </si>
   <si>
-    <t>LY01</t>
-  </si>
-  <si>
     <t>HA01</t>
   </si>
   <si>
-    <t>VIE1026.06</t>
-  </si>
-  <si>
     <t>VIE1026.07</t>
   </si>
   <si>
-    <t>Cở sở</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Tên Cơ sở</t>
-  </si>
-  <si>
-    <t>Hà Nội</t>
-  </si>
-  <si>
-    <t>Hồ Chí Minh</t>
-  </si>
-  <si>
-    <t>Cần Thơ</t>
-  </si>
-  <si>
-    <t>Đà Nẵng</t>
-  </si>
-  <si>
-    <t>Tây Nguyên</t>
-  </si>
-  <si>
-    <t>Hải Phòng</t>
-  </si>
-  <si>
-    <t>Hitech</t>
+    <t>Phòng</t>
+  </si>
+  <si>
+    <t>E201</t>
+  </si>
+  <si>
+    <t>Buổi thi</t>
+  </si>
+  <si>
+    <t>Giảng viên</t>
+  </si>
+  <si>
+    <t>Mô tả thi</t>
+  </si>
+  <si>
+    <t>Ngày học end</t>
+  </si>
+  <si>
+    <t>vinhndqph26105</t>
+  </si>
+  <si>
+    <t>GDCD</t>
+  </si>
+  <si>
+    <t>GDCD01</t>
+  </si>
+  <si>
+    <t>E203</t>
+  </si>
+  <si>
+    <t>vinhndqph26105hj</t>
+  </si>
+  <si>
+    <t>E204</t>
   </si>
 </sst>
 </file>
@@ -153,7 +143,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -161,35 +151,17 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,18 +476,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0AF609B-53F1-48E5-9D1F-42B9C4C94448}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="6" max="6" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -523,182 +499,270 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="4">
+        <v>45100</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="E2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4">
-        <v>45082</v>
-      </c>
-      <c r="C2" s="5">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="4">
+        <v>45100</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="4">
+        <v>45100</v>
+      </c>
+      <c r="B4" s="5">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="4">
+        <v>45100</v>
+      </c>
+      <c r="B5" s="5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="4">
+        <v>45100</v>
+      </c>
+      <c r="B6" s="5">
+        <v>5</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="4">
+        <v>45100</v>
+      </c>
+      <c r="B7" s="5">
+        <v>6</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="4">
+        <v>45100</v>
+      </c>
+      <c r="B8" s="5">
+        <v>3</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="4">
+        <v>45100</v>
+      </c>
+      <c r="B9" s="5">
+        <v>4</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="E9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4">
-        <v>45112</v>
-      </c>
-      <c r="C3" s="5">
-        <v>2</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4">
-        <v>45143</v>
-      </c>
-      <c r="C4" s="5">
-        <v>3</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="3">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBFD5E66-5723-4878-AF97-7B79D9531DD6}">
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="2" max="2" width="11.08984375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="6">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="6">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="6">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6" t="s">
+      <c r="I9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="6">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6" t="s">
+    <row r="10" spans="1:10">
+      <c r="A10" s="4">
+        <v>45100</v>
+      </c>
+      <c r="B10" s="5">
+        <v>5</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="6">
+      <c r="D10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="4">
+        <v>45100</v>
+      </c>
+      <c r="B11" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="6">
+      <c r="C11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>25</v>
+      <c r="J11" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>